<commit_message>
firebase'de geliştirilen Rack çizim uygulaması guncelleme
</commit_message>
<xml_diff>
--- a/templates/input_template_new.xlsx
+++ b/templates/input_template_new.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tarkancicek/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D65E6BE-84EF-314D-9301-C455BE70FCF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B6D5CC46-05B8-4A4A-A8C9-FBC600997848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3940" yWindow="2120" windowWidth="22260" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3940" yWindow="1620" windowWidth="22260" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Location" sheetId="20" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="85">
   <si>
     <t>U</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>K1-2A</t>
+  </si>
+  <si>
+    <t>K1-3A</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{32044C3A-E95C-8042-BF11-3A5340C5E87D}" name="Table1" displayName="Table1" ref="A1:U21" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{32044C3A-E95C-8042-BF11-3A5340C5E87D}" name="Table1" displayName="Table1" ref="A1:U21" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:U21" xr:uid="{32044C3A-E95C-8042-BF11-3A5340C5E87D}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -604,7 +607,7 @@
     <filterColumn colId="20" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{C6EE000A-3037-EE4E-9630-5525921D8E7D}" name="Corridor" dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{C6EE000A-3037-EE4E-9630-5525921D8E7D}" name="Corridor" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{23C4A128-B3F7-034F-8B20-6B37F489DFA0}" name="Cabinet1"/>
     <tableColumn id="3" xr3:uid="{4315BC4D-038E-E345-97BA-6574FC3F87D4}" name="Cabinet2"/>
     <tableColumn id="4" xr3:uid="{0D53E15E-4C0A-EC47-97FA-4D7941DF232E}" name="Cabinet3"/>
@@ -896,7 +899,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1019,7 +1022,7 @@
         <v>83</v>
       </c>
       <c r="D7" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -1107,7 +1110,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView zoomScale="135" zoomScaleNormal="135" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="C1" sqref="C1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1416,7 +1419,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>